<commit_message>
Agregando plantilla (inicial) sin información
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\Temporales\mantenimiento-priorizacion-vias\src\co\edu\udea\mantpriorivias\archivos\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -491,7 +491,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Código de la vía</t>
   </si>
@@ -637,12 +637,6 @@
     <t>Ejes equivalentes</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Cabezas Duras (88)</t>
   </si>
   <si>
@@ -652,37 +646,7 @@
     <t>Unidad</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>VIA2</t>
-  </si>
-  <si>
-    <t>VIA3</t>
-  </si>
-  <si>
-    <t>VIA4</t>
-  </si>
-  <si>
-    <t>VIA6</t>
-  </si>
-  <si>
-    <t>VIA7</t>
-  </si>
-  <si>
-    <t>VIA8</t>
-  </si>
-  <si>
     <t>Sección transversal Inapropiada (8H)</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>VIA9</t>
   </si>
 </sst>
 </file>
@@ -843,20 +807,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1217,15 +1181,9 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>150000</v>
-      </c>
-      <c r="B2" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="9"/>
     </row>
   </sheetData>
@@ -1236,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -1261,27 +1219,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="19" t="s">
         <v>14</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K1" s="17"/>
       <c r="L1" s="17"/>
@@ -1292,7 +1250,7 @@
       <c r="Q1" s="17"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="14" t="s">
         <v>36</v>
       </c>
@@ -1310,9 +1268,9 @@
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="I2" s="20"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>6</v>
@@ -1333,285 +1291,7 @@
         <v>11</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q12" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1667,7 +1347,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>21</v>
@@ -1726,7 +1406,7 @@
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1736,7 +1416,7 @@
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1424,7 @@
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1752,7 +1432,7 @@
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1760,7 +1440,7 @@
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
@@ -1768,7 +1448,7 @@
       <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="7" t="s">
         <v>32</v>
       </c>
@@ -1776,7 +1456,7 @@
       <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1784,7 +1464,7 @@
       <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>34</v>
       </c>
@@ -1792,7 +1472,7 @@
       <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Validación hoja Costos de mantenimiento
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\Temporales\mantenimiento-priorizacion-vias\src\co\edu\udea\mantpriorivias\archivos\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\Temporales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Presupuesto" sheetId="8" r:id="rId1"/>
-    <sheet name="Priorización" sheetId="9" r:id="rId2"/>
+    <sheet name="Presupuesto" sheetId="2" r:id="rId1"/>
+    <sheet name="Priorización" sheetId="1" r:id="rId2"/>
     <sheet name="Costos de mantenimiento" sheetId="5" r:id="rId3"/>
-    <sheet name="Factores de riesgo de la vía" sheetId="6" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="6" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -139,9 +139,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-&lt;200= 0,5
-entre 200 y 500 = 0,8
-&gt;500 = 1</t>
+&lt;100= 0,5
+entre 100 y 300 = 0,8
+&gt;300 = 1</t>
         </r>
       </text>
     </comment>
@@ -170,7 +170,61 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Samsung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+&lt;300= 0,5
+entre 300 y 500 = 0,8
+&gt;500 = 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Samsung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Definir porcentaje de daños en la vía:
+&lt;30%= 0,5
+entre 30% y 70% = 0,8
+&gt;70% = 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0">
+    <comment ref="M2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -225,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0">
+    <comment ref="O2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -252,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0">
+    <comment ref="P2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0">
+    <comment ref="Q2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -306,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0">
+    <comment ref="R2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -333,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0">
+    <comment ref="S2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -360,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0">
+    <comment ref="T2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,6 +435,60 @@
           </rPr>
           <t xml:space="preserve">
 ïndicar si es
+Bajo (L)
+Medio (M)
+Alto (H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Samsung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Indicar si es
+Baja (L)
+Media (M)
+Alta (H)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Samsung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Indicar si es
 Bajo (L)
 Medio (M)
 Alto (H)</t>
@@ -454,44 +562,8 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Samsung</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Samsung:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-&lt;7%
-Entre 7 y 12%
-&gt;12%</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Código de la vía</t>
   </si>
@@ -511,22 +583,7 @@
     <t>Desarrollo económico</t>
   </si>
   <si>
-    <t>Drenaje lateral inadecuado (82)</t>
-  </si>
-  <si>
-    <t>Corrugaciones (83)</t>
-  </si>
-  <si>
-    <t>Polvo (84)</t>
-  </si>
-  <si>
-    <t>Baches/Huecos (85)</t>
-  </si>
-  <si>
-    <t>Ahuellamiento/Surcos (86)</t>
-  </si>
-  <si>
-    <t>Agregado Suelto (87)</t>
+    <t>Sección transversal Inapropiada (81)</t>
   </si>
   <si>
     <t>Conectividad</t>
@@ -538,9 +595,6 @@
     <t>Vías alternas</t>
   </si>
   <si>
-    <t>Doble riego</t>
-  </si>
-  <si>
     <t>Micropavimento</t>
   </si>
   <si>
@@ -559,9 +613,6 @@
     <t>Valor unitario</t>
   </si>
   <si>
-    <t>Carpeta derodadura</t>
-  </si>
-  <si>
     <t>Slurry Seal</t>
   </si>
   <si>
@@ -571,9 +622,6 @@
     <t>Mecánica</t>
   </si>
   <si>
-    <t>Mantenimiento Tradicional</t>
-  </si>
-  <si>
     <t>Perfilado ligero, no contempla adición de material</t>
   </si>
   <si>
@@ -583,33 +631,9 @@
     <t xml:space="preserve">Corte de la base existente y  adición de agregado.  Incluye conformación y compactación </t>
   </si>
   <si>
-    <t>Limpieza de cunetas y obras de arte</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reconformar, construir, compactar y ampliar las cunetas</t>
-    </r>
-  </si>
-  <si>
-    <t>Construcción e instalación de sistemas de drenajes y alcantarillas</t>
-  </si>
-  <si>
     <t>Reaplicación localizada de grava</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cortar de base, adición de agregado y estabilizante, incluye conformación y compactación</t>
-  </si>
-  <si>
     <t>Perfilado y adición de materiales (agua y agregado, ó 50/50 mezcla de algún estabilizante con grava), incluye conformación y compactación</t>
   </si>
   <si>
@@ -628,33 +652,121 @@
     <t>Minero</t>
   </si>
   <si>
-    <t>Pendiente máxima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pluviosidad </t>
-  </si>
-  <si>
-    <t>Ejes equivalentes</t>
-  </si>
-  <si>
-    <t>Cabezas Duras (88)</t>
-  </si>
-  <si>
     <t>Daños presentes en la vía</t>
   </si>
   <si>
     <t>Unidad</t>
   </si>
   <si>
-    <t>Sección transversal Inapropiada (8H)</t>
+    <t>Personas transportadas por día</t>
+  </si>
+  <si>
+    <t>Tratamientos superficiales o riegos</t>
+  </si>
+  <si>
+    <t>Tratamiento superficial simple</t>
+  </si>
+  <si>
+    <t>Tratamiento superficial doble</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpieza de cunetas </t>
+  </si>
+  <si>
+    <t>conformación y ampliación de las cunetas</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenajes longitudinales</t>
+  </si>
+  <si>
+    <t>Construcción y ampliación de alcantarillas</t>
+  </si>
+  <si>
+    <t>Limpieza de alcantarillas y box culverts</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenajes transversales</t>
+  </si>
+  <si>
+    <t>Adición de agua</t>
+  </si>
+  <si>
+    <t>Adición de estabilizante control polvo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Corte de la base, adición de agregado y estabilizante control polvo, incluye conformación y compactación</t>
+  </si>
+  <si>
+    <t>Perfilado y revegetalización de taludes</t>
+  </si>
+  <si>
+    <t>Construcción de sistemas de drenaje para taludes</t>
+  </si>
+  <si>
+    <t>Estabilización de talud</t>
+  </si>
+  <si>
+    <t>Construcción de obra de contención para taludes</t>
+  </si>
+  <si>
+    <t>Construcción de lleno para estabilizar la banca</t>
+  </si>
+  <si>
+    <t>Construcción de obras de contención de la banca</t>
+  </si>
+  <si>
+    <t>Mantenimiento rutinario y periódico</t>
+  </si>
+  <si>
+    <t>Construcción de obras de disipación de energía</t>
+  </si>
+  <si>
+    <t>Nivelación y conformación de la banca</t>
+  </si>
+  <si>
+    <t>Drenaje Longitudinal inadecuado (82)</t>
+  </si>
+  <si>
+    <t>Drenaje Transversal Inadecuado (83)</t>
+  </si>
+  <si>
+    <t>Corrugaciones (84)</t>
+  </si>
+  <si>
+    <t>Polvo (85)</t>
+  </si>
+  <si>
+    <t>Baches/Huecos (86)</t>
+  </si>
+  <si>
+    <t>Ahuellamiento/Surcos (87)</t>
+  </si>
+  <si>
+    <t>Agregado Suelto (88)</t>
+  </si>
+  <si>
+    <t>Cabezas Duras (89)</t>
+  </si>
+  <si>
+    <t>Probabilidad de derrumbes (90)</t>
+  </si>
+  <si>
+    <t>Daños en la banca (91)</t>
+  </si>
+  <si>
+    <t>Indice de condición de la vía (URCI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -694,7 +806,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -754,16 +866,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -775,16 +921,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,14 +951,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -819,7 +989,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1154,7 +1324,8 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1164,139 +1335,173 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <sheetPr codeName="Hoja2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="20.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="16"/>
-    <col min="9" max="9" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="16"/>
-    <col min="14" max="14" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="20.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-    </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>44</v>
+      <c r="M2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J1:Q1"/>
+  <dataConsolidate/>
+  <mergeCells count="8">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:V1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:G2"/>
@@ -1304,32 +1509,43 @@
     <mergeCell ref="I1:I2"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:H1048576">
-      <formula1>"L,M,H"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="Q3:Q1048576">
-      <formula1>"S,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:P1048576">
-      <formula1>"L,M,H"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
       <formula1>"S,N"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:S1048576 U3:V1048576">
+      <formula1>"L,M,H"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576">
+      <formula1>"S,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576">
+      <formula1>"0,10,25,40,55,70,85,100"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja1!$A$1:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>J3:J1048576 B3:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja5"/>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1340,156 +1556,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
+      <c r="B26" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
+      <c r="B27" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
+      <c r="B29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31">
       <formula1>"m,m2,m3,Km,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1500,39 +1833,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja6">
-    <tabColor theme="3" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correcciones lectura de Costos de Mantenimiento
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andersson\Desktop\Temporales\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Presupuesto" sheetId="2" r:id="rId1"/>
-    <sheet name="Priorización" sheetId="1" r:id="rId2"/>
-    <sheet name="Costos de mantenimiento" sheetId="5" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="6" state="hidden" r:id="rId4"/>
+    <sheet name="Presupuesto" sheetId="1" r:id="rId1"/>
+    <sheet name="Priorización" sheetId="2" r:id="rId2"/>
+    <sheet name="Costos de mantenimiento" sheetId="3" r:id="rId3"/>
+    <sheet name="Valores posibles" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Samsung</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -40,7 +35,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -61,7 +56,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Samsung</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0">
@@ -74,7 +69,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -102,7 +97,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -129,7 +124,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -155,7 +150,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -180,7 +175,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -206,7 +201,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -234,7 +229,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -262,7 +257,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -289,7 +284,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -316,7 +311,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -343,7 +338,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -370,7 +365,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -397,7 +392,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -424,7 +419,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -451,7 +446,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -478,7 +473,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -502,10 +497,10 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Samsung</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -515,7 +510,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -533,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -543,7 +538,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samsung:</t>
+          <t>Autor:</t>
         </r>
         <r>
           <rPr>
@@ -563,210 +558,304 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+  <si>
+    <t>Presupuesto total inicial</t>
+  </si>
+  <si>
+    <t>% Administración</t>
+  </si>
+  <si>
+    <t>% Imprevistos</t>
+  </si>
+  <si>
+    <t>% Utilidades</t>
+  </si>
   <si>
     <t>Código de la vía</t>
   </si>
   <si>
-    <t>Presupuesto total inicial</t>
-  </si>
-  <si>
-    <t>% administración</t>
-  </si>
-  <si>
-    <t>% imprevistos</t>
-  </si>
-  <si>
-    <t>% utilidades</t>
-  </si>
-  <si>
     <t>Desarrollo económico</t>
   </si>
   <si>
+    <t>Conectividad</t>
+  </si>
+  <si>
+    <t>TPD</t>
+  </si>
+  <si>
+    <t>Vías alternas</t>
+  </si>
+  <si>
+    <t>Personas transportadas por día</t>
+  </si>
+  <si>
+    <t>Indice de condición de la vía (URCI)</t>
+  </si>
+  <si>
+    <t>Daños presentes en la vía</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>De servicios</t>
+  </si>
+  <si>
+    <t>Agropecuario</t>
+  </si>
+  <si>
+    <t>Minero</t>
+  </si>
+  <si>
     <t>Sección transversal Inapropiada (81)</t>
   </si>
   <si>
-    <t>Conectividad</t>
-  </si>
-  <si>
-    <t>TPD</t>
-  </si>
-  <si>
-    <t>Vías alternas</t>
+    <t>Drenaje Longitudinal inadecuado (82)</t>
+  </si>
+  <si>
+    <t>Drenaje Transversal Inadecuado (83)</t>
+  </si>
+  <si>
+    <t>Corrugaciones (84)</t>
+  </si>
+  <si>
+    <t>Polvo (85)</t>
+  </si>
+  <si>
+    <t>Baches/Huecos (86)</t>
+  </si>
+  <si>
+    <t>Ahuellamiento/Surcos (87)</t>
+  </si>
+  <si>
+    <t>Agregado Suelto (88)</t>
+  </si>
+  <si>
+    <t>Cabezas Duras (89)</t>
+  </si>
+  <si>
+    <t>Probabilidad de derrumbes (90)</t>
+  </si>
+  <si>
+    <t>Daños en la banca (91)</t>
+  </si>
+  <si>
+    <t>Tipo de mantenimiento</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Valor unitario</t>
+  </si>
+  <si>
+    <t>Tratamientos superficiales o riegos</t>
+  </si>
+  <si>
+    <t>ME1</t>
+  </si>
+  <si>
+    <t>Slurry Seal</t>
+  </si>
+  <si>
+    <t>ME2</t>
+  </si>
+  <si>
+    <t>Mapia</t>
+  </si>
+  <si>
+    <t>ME3</t>
   </si>
   <si>
     <t>Micropavimento</t>
   </si>
   <si>
-    <t>Mapia</t>
+    <t>ME4</t>
+  </si>
+  <si>
+    <t>Tratamiento superficial doble</t>
+  </si>
+  <si>
+    <t>ME5</t>
+  </si>
+  <si>
+    <t>Tratamiento superficial simple</t>
+  </si>
+  <si>
+    <t>Estabilización</t>
+  </si>
+  <si>
+    <t>ME6</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t>ME7</t>
   </si>
   <si>
     <t>Química</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Tipo de mantenimiento</t>
-  </si>
-  <si>
-    <t>Valor unitario</t>
-  </si>
-  <si>
-    <t>Slurry Seal</t>
-  </si>
-  <si>
-    <t>Estabilización</t>
+    <t>ME8</t>
   </si>
   <si>
     <t>Mecánica</t>
   </si>
   <si>
+    <t>Mantenimiento rutinario y periódico</t>
+  </si>
+  <si>
+    <t>MA1</t>
+  </si>
+  <si>
     <t>Perfilado ligero, no contempla adición de material</t>
   </si>
   <si>
+    <t>MA2</t>
+  </si>
+  <si>
     <t>Perfilado del terreno y adición de material</t>
   </si>
   <si>
+    <t>MA3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corte de la base existente y  adición de agregado.  Incluye conformación y compactación </t>
   </si>
   <si>
+    <t>MA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpieza de cunetas </t>
+  </si>
+  <si>
+    <t>MA5</t>
+  </si>
+  <si>
+    <t>MA6</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenajes longitudinales</t>
+  </si>
+  <si>
+    <t>MA7</t>
+  </si>
+  <si>
+    <t>Limpieza de alcantarillas y box culverts</t>
+  </si>
+  <si>
+    <t>MA8</t>
+  </si>
+  <si>
+    <t>Construcción y ampliación de alcantarillas</t>
+  </si>
+  <si>
+    <t>MA9</t>
+  </si>
+  <si>
+    <t>Construcción e instalación de sistemas de drenajes transversales</t>
+  </si>
+  <si>
+    <t>MA10</t>
+  </si>
+  <si>
+    <t>Adición de agua</t>
+  </si>
+  <si>
+    <t>MA11</t>
+  </si>
+  <si>
     <t>Reaplicación localizada de grava</t>
   </si>
   <si>
+    <t>MA12</t>
+  </si>
+  <si>
+    <t>Adición de estabilizante control polvo</t>
+  </si>
+  <si>
+    <t>MA13</t>
+  </si>
+  <si>
+    <t>Corte de la base, adición de agregado y estabilizante control polvo, incluye conformación y compactación</t>
+  </si>
+  <si>
+    <t>MA14</t>
+  </si>
+  <si>
     <t>Perfilado y adición de materiales (agua y agregado, ó 50/50 mezcla de algún estabilizante con grava), incluye conformación y compactación</t>
   </si>
   <si>
-    <t>Comercial</t>
-  </si>
-  <si>
-    <t>Industrial</t>
-  </si>
-  <si>
-    <t>De servicios</t>
-  </si>
-  <si>
-    <t>Agropecuario</t>
-  </si>
-  <si>
-    <t>Minero</t>
-  </si>
-  <si>
-    <t>Daños presentes en la vía</t>
-  </si>
-  <si>
-    <t>Unidad</t>
-  </si>
-  <si>
-    <t>Personas transportadas por día</t>
-  </si>
-  <si>
-    <t>Tratamientos superficiales o riegos</t>
-  </si>
-  <si>
-    <t>Tratamiento superficial simple</t>
-  </si>
-  <si>
-    <t>Tratamiento superficial doble</t>
-  </si>
-  <si>
-    <t>Física</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limpieza de cunetas </t>
-  </si>
-  <si>
-    <t>conformación y ampliación de las cunetas</t>
-  </si>
-  <si>
-    <t>Construcción e instalación de sistemas de drenajes longitudinales</t>
-  </si>
-  <si>
-    <t>Construcción y ampliación de alcantarillas</t>
-  </si>
-  <si>
-    <t>Limpieza de alcantarillas y box culverts</t>
-  </si>
-  <si>
-    <t>Construcción e instalación de sistemas de drenajes transversales</t>
-  </si>
-  <si>
-    <t>Adición de agua</t>
-  </si>
-  <si>
-    <t>Adición de estabilizante control polvo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Corte de la base, adición de agregado y estabilizante control polvo, incluye conformación y compactación</t>
+    <t>MA15</t>
   </si>
   <si>
     <t>Perfilado y revegetalización de taludes</t>
   </si>
   <si>
+    <t>MA16</t>
+  </si>
+  <si>
     <t>Construcción de sistemas de drenaje para taludes</t>
   </si>
   <si>
+    <t>MA17</t>
+  </si>
+  <si>
+    <t>Construcción de obras de disipación de energía</t>
+  </si>
+  <si>
+    <t>MA18</t>
+  </si>
+  <si>
     <t>Estabilización de talud</t>
   </si>
   <si>
+    <t>MA19</t>
+  </si>
+  <si>
     <t>Construcción de obra de contención para taludes</t>
   </si>
   <si>
+    <t>MA20</t>
+  </si>
+  <si>
+    <t>Nivelación y conformación de la banca</t>
+  </si>
+  <si>
+    <t>MA21</t>
+  </si>
+  <si>
     <t>Construcción de lleno para estabilizar la banca</t>
   </si>
   <si>
-    <t>Construcción de obras de contención de la banca</t>
-  </si>
-  <si>
-    <t>Mantenimiento rutinario y periódico</t>
-  </si>
-  <si>
-    <t>Construcción de obras de disipación de energía</t>
-  </si>
-  <si>
-    <t>Nivelación y conformación de la banca</t>
-  </si>
-  <si>
-    <t>Drenaje Longitudinal inadecuado (82)</t>
-  </si>
-  <si>
-    <t>Drenaje Transversal Inadecuado (83)</t>
-  </si>
-  <si>
-    <t>Corrugaciones (84)</t>
-  </si>
-  <si>
-    <t>Polvo (85)</t>
-  </si>
-  <si>
-    <t>Baches/Huecos (86)</t>
-  </si>
-  <si>
-    <t>Ahuellamiento/Surcos (87)</t>
-  </si>
-  <si>
-    <t>Agregado Suelto (88)</t>
-  </si>
-  <si>
-    <t>Cabezas Duras (89)</t>
-  </si>
-  <si>
-    <t>Probabilidad de derrumbes (90)</t>
-  </si>
-  <si>
-    <t>Daños en la banca (91)</t>
-  </si>
-  <si>
-    <t>Indice de condición de la vía (URCI)</t>
+    <t>MA22</t>
+  </si>
+  <si>
+    <t>Construcción de obra de contención para la banca</t>
+  </si>
+  <si>
+    <t>Conformación y ampliación de las cunetas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$$-240A]#,##0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -785,13 +874,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -907,90 +996,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,7 +1105,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1324,182 +1409,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="20.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="26"/>
+    <col min="9" max="9" width="12.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="27" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="27" customWidth="1"/>
+    <col min="13" max="13" width="21" style="27" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="27" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" style="27" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="27"/>
+    <col min="17" max="17" width="14.5703125" style="27" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" style="27" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="27"/>
+    <col min="21" max="21" width="14.7109375" style="27" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" style="27"/>
+    <col min="23" max="16384" width="11.42578125" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="27" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-    </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="6" t="s">
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+    </row>
+    <row r="2" spans="1:22" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="T2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="U2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="V2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>63</v>
-      </c>
     </row>
   </sheetData>
-  <dataConsolidate/>
   <mergeCells count="8">
-    <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:V1"/>
     <mergeCell ref="A1:A2"/>
@@ -1507,32 +1586,29 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576">
-      <formula1>"S,N"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:S1048576 U3:V1048576">
-      <formula1>"L,M,H"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576 T3:T1048576">
       <formula1>"S,N"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K1048576">
       <formula1>"0,10,25,40,55,70,85,100"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:S1048576 U3:V1048576">
+      <formula1>"L,M,H"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Hoja1!$A$1:$A$10</xm:f>
+            <xm:f>'Valores posibles'!$A$1:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:J1048576 B3:H1048576</xm:sqref>
+          <xm:sqref>B3:G1048576 H3:H1048576 J3:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1542,278 +1618,369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja5"/>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="17"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="19" t="s">
+      <c r="B10" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="17"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="18" t="s">
+      <c r="C10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="17"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1822,13 +1989,12 @@
     <mergeCell ref="A10:A31"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31">
-      <formula1>"m,m2,m3,Km,"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D31">
+      <formula1>"M,M2,M3,KM,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1837,63 +2003,62 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9">
+      <c r="A1" s="24">
         <v>0.1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="24">
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="24">
         <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="24">
         <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="24">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="24">
         <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="24">
         <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="24">
         <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="24">
         <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización de valores posibles
* Se actualizan todos aquellos valores posibles que iban de 0,1 a 1,0 para que vaya desde 0,0 hasta 1,0.
* Se corrije validación de URCI.
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="2" r:id="rId1"/>
@@ -970,7 +970,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1017,7 +1017,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -1184,9 +1184,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Hoja1!$A$1:$A$10</xm:f>
+            <xm:f>Hoja1!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:H1048576 J3:J1048576 K3:K1048576</xm:sqref>
+          <xm:sqref>B3:H1048576 J3:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1196,7 +1196,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1204,51 +1204,56 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios en plantilla de vías.
</commit_message>
<xml_diff>
--- a/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
+++ b/src/co/edu/udea/mantpriorivias/archivos/recursos/Plantilla_MantPriorVias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="2" r:id="rId1"/>
@@ -65,10 +65,10 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Para cada una de las áreas definir su importancia en la zona donde 
-Importancia Alta=[0,9-1]
-Importancia Media= [0,5-0,8]
-Importancia Baja= [0,1-0,4]
+Para cada una de las áreas, definir su importancia en la zona; donde: 
+Importancia Alta=[0,8-1]
+Importancia Media= [0,4-0,7]
+Importancia Baja= [0,0-0,3]
 </t>
         </r>
       </text>
@@ -84,9 +84,9 @@
           </rPr>
           <t xml:space="preserve">
 Número de cabeceras municipales o poblados que conecta la vía
-2 =  [0,1-0,4]
-entre 2 y 5 = [0,5-0,8]
-&gt;5 = [0,9-1]
+2 =  [0,0-0,3]
+entre 2 y 5 = [0,4-0,7]
+&gt;5 = [0,8-1]
 </t>
         </r>
       </text>
@@ -100,10 +100,10 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-&lt;200= [0,1-04]
-entre 200 y 500 = [0,5-0,8]
-&gt;500 = [0,9-1]
+          <t xml:space="preserve">Tránsito promedio diario:
+&lt;200= [0,0-0,3]
+entre 200 y 500 = [0,4-0,7]
+&gt;500 = [0,8-1]
 </t>
         </r>
       </text>
@@ -133,9 +133,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-&lt;500= [0,1-0,4]
-entre 500 y 800 = [0,5-0,8]
-&gt;800 = [0,9-1]</t>
+&lt;500= [0,0-0,3]
+entre 500 y 800 = [0,4-0,7]
+&gt;800 = [0,8-1,0]</t>
         </r>
       </text>
     </comment>
@@ -151,9 +151,9 @@
           <t xml:space="preserve">
 Este parámetro se evaluará de acuerdo a la escala de URCI, para ello hay que realizar todo el procedimiento descrito en el manual del URCI (Indice de condeción de las vías no pavimentadas), y se calificará de acuerdo a lo siguiente:
 Valor URCI          Calificación
-0-40                     [0,9-1]
-41-70                   [0,5-0,8]
-71-100                 [0,1-0,4]
+0-40                     [0,8-1,0]
+41-70                   [0,4-0,7]
+71-100                 [0,0-0,3]
 </t>
         </r>
       </text>
@@ -970,7 +970,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1017,7 +1017,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>